<commit_message>
fix: electricity consumption divided by 6
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="5">
   <si>
     <t>ID_Activity</t>
   </si>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,153 +470,153 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2">
-        <v>0.15529999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>0.11210000000000001</v>
+        <v>0.35709999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>0.18729999999999999</v>
+        <v>0.1429</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>0.1221</v>
+        <v>7.1400000000000005E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>0.19339999999999999</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>0.2298</v>
+        <v>0.17860000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="2">
-        <v>0.35709999999999997</v>
+        <v>0.37030000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2">
-        <v>0.1429</v>
+        <v>6.0199999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2">
-        <v>7.1400000000000005E-2</v>
+        <v>0.28260000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2">
-        <v>0.25</v>
+        <v>3.7100000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="2">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="2">
-        <v>0.17860000000000001</v>
+        <v>3.3099999999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -624,13 +624,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="2">
-        <v>0.37030000000000002</v>
+        <v>5.5399999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -638,13 +638,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="2">
-        <v>6.0199999999999997E-2</v>
+        <v>3.61E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -652,13 +652,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="2">
-        <v>0.28260000000000002</v>
+        <v>5.7200000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -666,195 +666,195 @@
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="2">
-        <v>3.7100000000000001E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2">
-        <v>3.3099999999999997E-2</v>
+        <v>0.76600000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="2">
-        <v>5.5399999999999998E-2</v>
+        <v>0.23400000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="2">
-        <v>3.61E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="2">
-        <v>5.7200000000000001E-2</v>
+        <v>0.23250000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="2">
-        <v>6.8000000000000005E-2</v>
+        <v>0.53500000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="2">
-        <v>0.76600000000000001</v>
+        <v>0.23250000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="2">
-        <v>0.23400000000000001</v>
+        <v>0.66710000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2">
-        <v>1</v>
+        <v>0.33289999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="2">
-        <v>0.23250000000000001</v>
+        <v>9.11E-2</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="2">
-        <v>0.53500000000000003</v>
+        <v>0.16020000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="2">
-        <v>0.23250000000000001</v>
+        <v>0.1167</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="2">
-        <v>0.66710000000000003</v>
+        <v>0.20810000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="2">
-        <v>0.33289999999999997</v>
+        <v>4.07E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -862,13 +862,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="2">
-        <v>9.11E-2</v>
+        <v>0.20469999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -876,13 +876,13 @@
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="2">
-        <v>0.16020000000000001</v>
+        <v>1.04E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -890,13 +890,13 @@
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="2">
-        <v>0.1167</v>
+        <v>0.11459999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -904,265 +904,265 @@
         <v>9</v>
       </c>
       <c r="B34" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="2">
-        <v>0.20810000000000001</v>
+        <v>5.3499999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>9</v>
-      </c>
-      <c r="B35" s="2">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="2">
-        <v>4.07E-2</v>
+      <c r="D35" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D36" s="2">
-        <v>0.20469999999999999</v>
+        <v>0.26119999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B37" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="2">
-        <v>1.04E-2</v>
+        <v>0.4597</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="2">
-        <v>0.11459999999999999</v>
+        <v>6.6900000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="2">
-        <v>5.3499999999999999E-2</v>
+        <v>0.1195</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>10</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="B40" s="2">
+        <v>6</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="3">
-        <v>1</v>
+      <c r="D40" s="2">
+        <v>9.2700000000000005E-2</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>11</v>
-      </c>
-      <c r="B41" s="2">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.26119999999999999</v>
+      <c r="D41" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>11</v>
-      </c>
-      <c r="B42" s="2">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.4597</v>
+      <c r="D42" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>11</v>
-      </c>
-      <c r="B43" s="2">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="2">
-        <v>6.6900000000000001E-2</v>
+      <c r="D43" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>11</v>
-      </c>
-      <c r="B44" s="2">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.1195</v>
+      <c r="D44" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B45" s="2">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="2">
-        <v>9.2700000000000005E-2</v>
+      <c r="D45" s="4">
+        <v>0.53046670162558995</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>12</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B46" s="2">
+        <v>35</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="3">
-        <v>1</v>
+      <c r="D46" s="4">
+        <v>0.22338751966439432</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>13</v>
-      </c>
-      <c r="B47" s="3">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="B47" s="2">
+        <v>36</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="3">
-        <v>1</v>
+      <c r="D47" s="4">
+        <v>0.24614577871001572</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>14</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B48" s="2">
+        <v>5</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="3">
-        <v>1</v>
+      <c r="D48" s="2">
+        <v>0.18529999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>15</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B49" s="2">
+        <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="3">
-        <v>1</v>
+      <c r="D49" s="2">
+        <v>0.14419999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B50" s="2">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D50" s="4">
-        <v>0.53046670162558995</v>
+      <c r="D50" s="2">
+        <v>0.10390000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B51" s="2">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="4">
-        <v>0.22338751966439432</v>
+      <c r="D51" s="2">
+        <v>0.17380000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B52" s="2">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="4">
-        <v>0.24614577871001572</v>
+      <c r="D52" s="2">
+        <v>0.17949999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1170,82 +1170,12 @@
         <v>17</v>
       </c>
       <c r="B53" s="2">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D53" s="2">
-        <v>0.18529999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>17</v>
-      </c>
-      <c r="B54" s="2">
-        <v>14</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.14419999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>17</v>
-      </c>
-      <c r="B55" s="2">
-        <v>17</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="2">
-        <v>0.10390000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>17</v>
-      </c>
-      <c r="B56" s="2">
-        <v>18</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="2">
-        <v>0.17380000000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>17</v>
-      </c>
-      <c r="B57" s="2">
-        <v>20</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0.17949999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>17</v>
-      </c>
-      <c r="B58" s="2">
-        <v>21</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="2">
         <v>0.21329999999999999</v>
       </c>
     </row>
@@ -1255,26 +1185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4511c60809de47fd61668c7a2fa421c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="113b7667aea05225525c2a1f4252ac59" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1479,10 +1389,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D125F7-70BC-4CD8-BA77-1F77C7034327}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
+    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1499,20 +1440,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D125F7-70BC-4CD8-BA77-1F77C7034327}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
-    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revised technology trigger probabilities.
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\FLEX\data\input_behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8E496D-6BEE-0D40-B5BA-09C0361F764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2985" windowWidth="26535" windowHeight="13095"/>
+    <workbookView xWindow="6100" yWindow="-28300" windowWidth="17060" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="5">
   <si>
     <t>ID_Activity</t>
   </si>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -103,12 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,22 +425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -465,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -479,625 +482,640 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>0.35709999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>0.1429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.35709999999999997</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>7.1400000000000005E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.1429</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" s="2">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
         <v>29</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.17860000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>4</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.37030000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.30030000000000001</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
         <v>6.0199999999999997E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.28260000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.25259999999999999</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
         <v>16</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2">
         <v>3.7100000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
         <v>17</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2">
         <v>3.3099999999999997E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2">
         <v>5.5399999999999998E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2">
         <v>19</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2">
         <v>3.61E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2">
         <v>5.7200000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>4</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
         <v>6.8000000000000005E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B20" s="2">
         <v>15</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B21" s="2">
         <v>25</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>6</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2">
         <v>30</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
         <v>22</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.23250000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.20250000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>7</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B26" s="2">
         <v>23</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.53500000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>7</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B27" s="2">
         <v>24</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.23250000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="C27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.20250000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>8</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B28" s="2">
         <v>32</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.66710000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>8</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B29" s="2">
         <v>33</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2">
         <v>0.33289999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>9.11E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>9</v>
-      </c>
-      <c r="B27" s="2">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.16020000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.1167</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.20810000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="2">
-        <v>4.07E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>9.11E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="2">
-        <v>0.20469999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.16020000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="2">
-        <v>1.04E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.1167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="2">
-        <v>0.11459999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.20810000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>9</v>
       </c>
       <c r="B34" s="2">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4.07E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>9</v>
+      </c>
+      <c r="B35" s="2">
+        <v>7</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.20469999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>9</v>
+      </c>
+      <c r="B36" s="2">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1.04E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.11459999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>9</v>
+      </c>
+      <c r="B38" s="2">
         <v>10</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="2">
         <v>5.3499999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>10</v>
       </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>11</v>
-      </c>
-      <c r="B36" s="2">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.26119999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>11</v>
-      </c>
-      <c r="B37" s="2">
-        <v>3</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.4597</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>11</v>
-      </c>
-      <c r="B38" s="2">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="2">
-        <v>6.6900000000000001E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>11</v>
-      </c>
-      <c r="B39" s="2">
-        <v>5</v>
+      <c r="B39" s="3">
+        <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.1195</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>11</v>
       </c>
       <c r="B40" s="2">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.26119999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>11</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.4597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>11</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <v>6.6900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>11</v>
+      </c>
+      <c r="B43" s="2">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.1195</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>11</v>
+      </c>
+      <c r="B44" s="2">
         <v>6</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="C44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="2">
         <v>9.2700000000000005E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B41" s="3">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>13</v>
-      </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>14</v>
-      </c>
-      <c r="B43" s="3">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>15</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>16</v>
-      </c>
       <c r="B45" s="2">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="4">
-        <v>0.53046670162558995</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <v>0.26119999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B46" s="2">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D46" s="4">
-        <v>0.22338751966439432</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <v>0.4597</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B47" s="2">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="4">
-        <v>0.24614577871001572</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <v>6.6900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B48" s="2">
         <v>5</v>
@@ -1106,77 +1124,218 @@
         <v>4</v>
       </c>
       <c r="D48" s="2">
-        <v>0.18529999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.1195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
+        <v>12</v>
+      </c>
+      <c r="B49" s="2">
+        <v>6</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="2">
+        <v>9.2700000000000005E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>13</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>14</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>15</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>16</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>16</v>
+      </c>
+      <c r="B54" s="2">
+        <v>34</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>16</v>
+      </c>
+      <c r="B55" s="2">
+        <v>35</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0.18338751966439401</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>16</v>
+      </c>
+      <c r="B56" s="2">
+        <v>36</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0.20561457787100099</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
         <v>17</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B57" s="2">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>17</v>
+      </c>
+      <c r="B58" s="2">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.23530000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>17</v>
+      </c>
+      <c r="B59" s="2">
         <v>14</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.14419999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="C59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.1042</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
         <v>17</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B60" s="2">
         <v>17</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="2">
-        <v>0.10390000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="C60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <v>9.3899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
         <v>17</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B61" s="2">
         <v>18</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.17380000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="C61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="2">
+        <v>9.3799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
         <v>17</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B62" s="2">
         <v>20</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0.17949999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="C62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.16950000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
         <v>17</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B63" s="2">
         <v>21</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0.21329999999999999</v>
+      <c r="C63" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.20330000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revised technology trigger probabilities."
This reverts commit 1c3b92b4d27a9eb18d46112fec4640904c3982dd.
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/PycharmProjects/FLEX/data/input_behavior/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315B6688-08BE-EE40-A9A1-98F6D8CB8536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D8E496D-6BEE-0D40-B5BA-09C0361F764B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10960" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6100" yWindow="-28300" windowWidth="17060" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,12 +79,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,10 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -421,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17:L18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,13 +991,13 @@
       <c r="A39" s="2">
         <v>10</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1138,13 +1145,13 @@
       <c r="A50" s="2">
         <v>13</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="3">
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1152,13 +1159,13 @@
       <c r="A51" s="2">
         <v>14</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="3">
         <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1166,13 +1173,13 @@
       <c r="A52" s="2">
         <v>15</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1180,16 +1187,16 @@
       <c r="A53" s="2">
         <v>16</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="3">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="3">
         <v>0.1</v>
       </c>
-      <c r="G53" s="4"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
@@ -1201,7 +1208,7 @@
       <c r="C54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>0.51100000000000001</v>
       </c>
     </row>
@@ -1215,7 +1222,7 @@
       <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>0.18338751966439401</v>
       </c>
     </row>
@@ -1229,7 +1236,7 @@
       <c r="C56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>0.20561457787100099</v>
       </c>
     </row>
@@ -1243,7 +1250,7 @@
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="4">
         <v>0.1</v>
       </c>
     </row>
@@ -1542,15 +1549,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
@@ -1559,6 +1557,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1581,14 +1588,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E8BF163-7E87-4B8A-965E-CB930C72B92B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1597,4 +1596,12 @@
     <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Calibration of Technology trigger probabilities, building parameters and implementation of changes.
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_TriggerProbability.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevanskorna/PycharmProjects/FLEX/data/input_behavior/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB9E2DA-CA94-D048-A400-D663AF74C7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F58EF3-BFEE-9840-BB21-381376048B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1880" yWindow="-20700" windowWidth="15820" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="-28300" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="5">
   <si>
     <t>ID_Activity</t>
   </si>
@@ -242,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}" name="Table1" displayName="Table1" ref="A1:D66" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D66" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}" name="Table1" displayName="Table1" ref="A1:D58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D58" xr:uid="{5DEDA1C4-9DD0-5445-B0A4-9BFEFCA653EF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D13772B6-3362-0E4E-85D9-C4A4391AA10A}" name="ID_Activity" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{A6DBB581-D6B6-FE40-937D-2BF0BA88D4B1}" name="ID_Technology" dataDxfId="2"/>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,27 +612,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4">
-        <v>0.1</v>
-      </c>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4">
-        <v>0.3</v>
+        <v>0.11111111111111112</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -641,13 +642,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>0.1</v>
+        <v>0.11111111111111112</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -656,13 +657,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4">
-        <v>0.1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -671,43 +672,43 @@
         <v>3</v>
       </c>
       <c r="B8" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>0.29659259259259263</v>
+      </c>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>4</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4">
-        <v>0.1</v>
+        <v>0.17056790123456775</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -716,13 +717,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="4">
-        <v>0.26693333333333336</v>
+        <v>0.2494814814814815</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -731,13 +732,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4">
-        <v>0.15351111111111099</v>
+        <v>3.6641975308641973E-2</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -746,13 +747,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="4">
-        <v>0.22453333333333336</v>
+        <v>3.2691358024691357E-2</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -761,13 +762,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="4">
-        <v>3.2977777777777779E-2</v>
+        <v>5.4716049382716049E-2</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -776,13 +777,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="4">
-        <v>2.9422222222222225E-2</v>
+        <v>3.5654320987654323E-2</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -791,13 +792,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4">
-        <v>4.9244444444444445E-2</v>
+        <v>5.649382716049383E-2</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -806,353 +807,367 @@
         <v>4</v>
       </c>
       <c r="B17" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="4">
-        <v>3.2088888888888889E-2</v>
+        <v>6.7160493827160495E-2</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="4">
-        <v>5.0844444444444449E-2</v>
+        <v>0.4</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4">
-        <v>6.0444444444444446E-2</v>
+        <v>0.6</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D21" s="4">
-        <v>0.2</v>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="4">
-        <v>0.6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="4">
-        <v>0.5</v>
-      </c>
+        <v>0.8</v>
+      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24" s="2">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="4">
-        <v>0.3</v>
-      </c>
+        <v>0.21361820199778001</v>
+      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B26" s="2">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="4">
-        <v>0.7</v>
-      </c>
+        <v>0.124461709211987</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="4">
-        <v>0.1</v>
-      </c>
+        <v>9.0665926748057679E-2</v>
+      </c>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="4">
-        <v>0.8</v>
-      </c>
+        <v>0.16167591564927855</v>
+      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="2">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="4">
-        <v>0.1</v>
-      </c>
+        <v>3.1620421753607089E-2</v>
+      </c>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>9</v>
       </c>
       <c r="B30" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.159034406215316</v>
+      </c>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>9</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="4">
-        <v>0.19247</v>
-      </c>
-      <c r="F31" s="7"/>
+        <v>6.3573806881243047E-2</v>
+      </c>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>9</v>
       </c>
       <c r="B32" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="4">
-        <v>0.11214000000000002</v>
-      </c>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.145528301886792</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>9</v>
       </c>
       <c r="B33" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="4">
-        <v>8.1689999999999985E-2</v>
-      </c>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>9.7114317425083235E-3</v>
+      </c>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>9</v>
-      </c>
-      <c r="B34" s="2">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>11</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>11</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.24444444444444438</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>11</v>
+      </c>
+      <c r="B37" s="2">
+        <v>3</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>11</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="4">
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2">
         <v>5</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0.14566999999999999</v>
-      </c>
-      <c r="F34" s="7"/>
-    </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
-        <v>9</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="C39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>11</v>
+      </c>
+      <c r="B40" s="2">
         <v>6</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="4">
-        <v>2.8489999999999994E-2</v>
-      </c>
-      <c r="F35" s="7"/>
-    </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>9</v>
-      </c>
-      <c r="B36" s="2">
-        <v>7</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0.14329</v>
-      </c>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>9</v>
-      </c>
-      <c r="B37" s="2">
-        <v>8</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="4">
-        <v>5.7279999999999998E-2</v>
-      </c>
-      <c r="F37" s="7"/>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>9</v>
-      </c>
-      <c r="B38" s="2">
-        <v>9</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.13022</v>
-      </c>
-      <c r="F38" s="7"/>
-    </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>9</v>
-      </c>
-      <c r="B39" s="2">
-        <v>10</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="4">
-        <v>8.7500000000000008E-3</v>
-      </c>
-      <c r="F39" s="7"/>
-    </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>10</v>
-      </c>
-      <c r="B40" s="3">
-        <v>1</v>
-      </c>
       <c r="C40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D40" s="4">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
@@ -1161,12 +1176,14 @@
         <v>4</v>
       </c>
       <c r="D41" s="6">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42" s="2">
         <v>2</v>
@@ -1175,12 +1192,13 @@
         <v>4</v>
       </c>
       <c r="D42" s="4">
-        <v>5.8959999999999999E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.24444444444444438</v>
+      </c>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43" s="2">
         <v>3</v>
@@ -1189,12 +1207,13 @@
         <v>4</v>
       </c>
       <c r="D43" s="4">
-        <v>0.51776</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44" s="2">
         <v>4</v>
@@ -1203,12 +1222,13 @@
         <v>4</v>
       </c>
       <c r="D44" s="4">
-        <v>5.3520000000000005E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B45" s="2">
         <v>5</v>
@@ -1217,12 +1237,13 @@
         <v>4</v>
       </c>
       <c r="D45" s="4">
-        <v>9.5600000000000004E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B46" s="2">
         <v>6</v>
@@ -1231,289 +1252,235 @@
         <v>4</v>
       </c>
       <c r="D46" s="4">
-        <v>7.4160000000000004E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>12</v>
-      </c>
-      <c r="B47" s="2">
+        <v>13</v>
+      </c>
+      <c r="B47" s="3">
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D47" s="6">
+        <v>1</v>
+      </c>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>12</v>
-      </c>
-      <c r="B48" s="2">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="4">
-        <v>0.2306</v>
-      </c>
+      <c r="D48" s="6">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>12</v>
-      </c>
-      <c r="B49" s="2">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="4">
-        <v>0.27984999999999999</v>
-      </c>
+      <c r="D49" s="6">
+        <v>1</v>
+      </c>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B50" s="2">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D50" s="4">
-        <v>8.3449999999999996E-2</v>
-      </c>
+        <v>0.46241872444730292</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B51" s="2">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D51" s="4">
-        <v>5.9749999999999998E-2</v>
-      </c>
+        <v>0.34690222387026892</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B52" s="2">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="4">
-        <v>4.6350000000000002E-2</v>
-      </c>
+        <v>0.1906790516824281</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>13</v>
-      </c>
-      <c r="B53" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B53" s="2">
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="6">
-        <v>1</v>
-      </c>
+      <c r="D53" s="4">
+        <v>0.41666666666666657</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
+        <v>17</v>
+      </c>
+      <c r="B54" s="2">
         <v>14</v>
       </c>
-      <c r="B54" s="3">
-        <v>1</v>
-      </c>
       <c r="C54" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D54" s="6">
-        <v>1</v>
-      </c>
+      <c r="D54" s="4">
+        <v>0.1148680273473412</v>
+      </c>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>15</v>
-      </c>
-      <c r="B55" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B55" s="2">
+        <v>17</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D55" s="6">
-        <v>1</v>
-      </c>
+      <c r="D55" s="4">
+        <v>7.8481520485432013E-2</v>
+      </c>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>16</v>
-      </c>
-      <c r="B56" s="3">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B56" s="2">
+        <v>18</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="6">
-        <v>0.82</v>
-      </c>
-      <c r="G56" s="5"/>
+      <c r="D56" s="4">
+        <v>7.8397940591411308E-2</v>
+      </c>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B57" s="2">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D57" s="4">
-        <v>0.1022</v>
-      </c>
+        <v>0.14166792036507697</v>
+      </c>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B58" s="2">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D58" s="4">
-        <v>3.6677503932878809E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
-        <v>16</v>
-      </c>
-      <c r="B59" s="2">
-        <v>34</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D59" s="4">
-        <v>4.1122915574200197E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>17</v>
-      </c>
-      <c r="B60" s="2">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D60" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
-        <v>17</v>
-      </c>
-      <c r="B61" s="2">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
-        <v>17</v>
-      </c>
-      <c r="B62" s="2">
-        <v>14</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="4">
-        <v>6.2704979690085746E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>17</v>
-      </c>
-      <c r="B63" s="2">
-        <v>17</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D63" s="4">
-        <v>5.6506694749511054E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="2">
-        <v>17</v>
-      </c>
-      <c r="B64" s="2">
-        <v>18</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="4">
-        <v>5.6446517225816145E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="2">
-        <v>17</v>
-      </c>
-      <c r="B65" s="2">
-        <v>20</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D65" s="4">
-        <v>0.10200090266285543</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
-        <v>17</v>
-      </c>
-      <c r="B66" s="2">
-        <v>21</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="4">
-        <v>0.1223409056717316</v>
-      </c>
+        <v>0.16991792454407165</v>
+      </c>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1524,15 +1491,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
@@ -1543,7 +1501,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4511c60809de47fd61668c7a2fa421c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="113b7667aea05225525c2a1f4252ac59" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1748,15 +1706,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E8BF163-7E87-4B8A-965E-CB930C72B92B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1767,7 +1726,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D125F7-70BC-4CD8-BA77-1F77C7034327}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1784,4 +1743,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD38B489-F981-428C-BF72-292671E2847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>